<commit_message>
Updated PKIX.20 test parameters
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/PIV-I-GSA_MSO_Cards.xlsx
+++ b/conformancelib/testdata/PIV-I-GSA_MSO_Cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\bf7450\git\piv-conformance\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F431A46B-B22B-4137-B769-1F8C871CD7AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B804AC3-2EBB-4B2D-97DC-B57A6CE40838}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Steps Overview" sheetId="1" r:id="rId1"/>
@@ -3752,9 +3752,6 @@
     <t>Confirm id-PIV-cardAuth exists in extendedKeyUsage extension and does not assert any other OIDs</t>
   </si>
   <si>
-    <t>CARD_HOLDER_UNIQUE_IDENTIFIER_OID:2.16.840.1.101.3.6.7,X509_CERTIFICATE_FOR_CARD_AUTHENTICATION_OID:2.16.840.1.101.3.6.7</t>
-  </si>
-  <si>
     <t>Card Auth id-PIV-cardAuth EKU keyPurposeID OID</t>
   </si>
   <si>
@@ -3831,6 +3828,9 @@
   </si>
   <si>
     <t>CAT:SLEEPY, DOG:HUNGRY, ELEPHANT:SAD</t>
+  </si>
+  <si>
+    <t>X509_CERTIFICATE_FOR_CARD_AUTHENTICATION_OID:2.16.840.1.101.3.6.8,CARD_HOLDER_UNIQUE_IDENTIFIER_OID:2.16.840.1.101.3.8.7</t>
   </si>
 </sst>
 </file>
@@ -3840,7 +3840,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -3872,6 +3872,11 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -3912,7 +3917,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -4269,11 +4274,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4446,6 +4466,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -43025,8 +43048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:IU29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -48408,14 +48431,14 @@
       <c r="D21" s="13" t="s">
         <v>1240</v>
       </c>
-      <c r="E21" s="13" t="s">
-        <v>1241</v>
+      <c r="E21" s="64" t="s">
+        <v>1267</v>
       </c>
       <c r="F21" s="13" t="s">
         <v>880</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="H21" s="39"/>
       <c r="I21" s="30"/>
@@ -48668,25 +48691,25 @@
     </row>
     <row r="22" spans="1:255" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="B22" s="13" t="s">
         <v>1193</v>
       </c>
       <c r="C22" s="13" t="s">
+        <v>1243</v>
+      </c>
+      <c r="D22" s="13" t="s">
         <v>1244</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="E22" s="13" t="s">
         <v>1245</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>1246</v>
       </c>
       <c r="F22" s="13" t="s">
         <v>896</v>
       </c>
       <c r="G22" s="13" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="H22" s="39"/>
       <c r="I22" s="30"/>
@@ -48945,7 +48968,7 @@
         <v>1193</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="D23" s="13" t="s">
         <v>706</v>
@@ -49210,7 +49233,7 @@
         <v>1193</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="D24" s="13" t="s">
         <v>711</v>
@@ -49475,13 +49498,13 @@
         <v>1193</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="D25" s="13" t="s">
         <v>700</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
@@ -49742,7 +49765,7 @@
         <v>1193</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="D26" s="13" t="s">
         <v>713</v>
@@ -50007,7 +50030,7 @@
         <v>1193</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="D27" s="13" t="s">
         <v>851</v>
@@ -50272,7 +50295,7 @@
         <v>1193</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="D28" s="13" t="s">
         <v>686</v>
@@ -50282,7 +50305,7 @@
       </c>
       <c r="F28" s="13"/>
       <c r="G28" s="13" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="H28" s="39"/>
       <c r="I28" s="30"/>
@@ -50541,10 +50564,10 @@
         <v>1193</v>
       </c>
       <c r="C29" s="13" t="s">
+        <v>1255</v>
+      </c>
+      <c r="D29" s="13" t="s">
         <v>1256</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>1257</v>
       </c>
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
@@ -51100,20 +51123,20 @@
         <v>293</v>
       </c>
       <c r="B2" s="13" t="s">
+        <v>1257</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>1258</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="D2" s="13" t="s">
         <v>1259</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>1260</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="13" t="s">
         <v>880</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="H2" s="59"/>
       <c r="I2" s="60"/>
@@ -51366,19 +51389,19 @@
     </row>
     <row r="3" spans="1:255" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
+        <v>1261</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>1257</v>
+      </c>
+      <c r="C3" s="13" t="s">
         <v>1262</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>1258</v>
-      </c>
-      <c r="C3" s="13" t="s">
+      <c r="D3" s="13" t="s">
+        <v>1259</v>
+      </c>
+      <c r="E3" s="13" t="s">
         <v>1263</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>1260</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>1264</v>
       </c>
       <c r="F3" s="13" t="s">
         <v>896</v>
@@ -51635,19 +51658,19 @@
     </row>
     <row r="4" spans="1:255" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
+        <v>1264</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>1257</v>
+      </c>
+      <c r="C4" s="13" t="s">
         <v>1265</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>1258</v>
-      </c>
-      <c r="C4" s="13" t="s">
+      <c r="D4" s="13" t="s">
+        <v>1259</v>
+      </c>
+      <c r="E4" s="13" t="s">
         <v>1266</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>1260</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>1267</v>
       </c>
       <c r="F4" s="13" t="s">
         <v>896</v>

</xml_diff>

<commit_message>
Updated wording in 10.3.1.9
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/PIV-I-GSA_MSO_Cards.xlsx
+++ b/conformancelib/testdata/PIV-I-GSA_MSO_Cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\bf7450\git\piv-conformance\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B804AC3-2EBB-4B2D-97DC-B57A6CE40838}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E7FC2F-E214-4B72-98EE-599FB210BAAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Steps Overview" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2977" uniqueCount="1268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2977" uniqueCount="1269">
   <si>
     <t>Document</t>
   </si>
@@ -3831,6 +3831,9 @@
   </si>
   <si>
     <t>X509_CERTIFICATE_FOR_CARD_AUTHENTICATION_OID:2.16.840.1.101.3.6.8,CARD_HOLDER_UNIQUE_IDENTIFIER_OID:2.16.840.1.101.3.8.7</t>
+  </si>
+  <si>
+    <t>Message digest from signed attributes bag matches the digest over Facial Imagbe biometric data (excluding contents of digital signature field)</t>
   </si>
 </sst>
 </file>
@@ -5633,8 +5636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IV473"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A354" workbookViewId="0">
-      <selection activeCell="C356" sqref="C356"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A294" workbookViewId="0">
+      <selection activeCell="C306" sqref="C306"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -10916,7 +10919,7 @@
         <v>594</v>
       </c>
       <c r="C306" s="8" t="s">
-        <v>566</v>
+        <v>1268</v>
       </c>
       <c r="D306" s="9" t="s">
         <v>530</v>
@@ -43048,7 +43051,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:IU29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C13" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C13" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated CMS.5 with parameter list
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/PIV-I-GSA_MSO_Cards.xlsx
+++ b/conformancelib/testdata/PIV-I-GSA_MSO_Cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\bf7450\git\piv-conformance\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0A6BD3-0D01-4B08-B907-C575FB1C347F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F430BCB-6029-4378-94B5-FACEE0ED1A35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="23040" windowHeight="12360" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="23040" windowHeight="12360" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Steps Overview" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2982" uniqueCount="1272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2983" uniqueCount="1273">
   <si>
     <t>Document</t>
   </si>
@@ -3843,6 +3843,9 @@
   </si>
   <si>
     <t>6</t>
+  </si>
+  <si>
+    <t>CARD_HOLDER_UNIQUE_IDENTIFIER_OID:2.16.840.1.101.3.6.1,CARDHOLDER_FINGERPRINTS_OID:2.16.840.1.101.3.6.2,CARDHOLDER_FACIAL_IMAGE_OID:2.16.840.1.101.3.6.2,CARDHOLDER_IRIS_IMAGES_OID:2.16.840</t>
   </si>
 </sst>
 </file>
@@ -14057,7 +14060,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:IU56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -42411,7 +42414,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:IV30"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -42537,7 +42542,9 @@
       <c r="D6" s="13" t="s">
         <v>1124</v>
       </c>
-      <c r="E6" s="13"/>
+      <c r="E6" s="13" t="s">
+        <v>1272</v>
+      </c>
       <c r="F6" s="13" t="s">
         <v>879</v>
       </c>

</xml_diff>